<commit_message>
acceso problemas ejemplo y dragon ball
</commit_message>
<xml_diff>
--- a/courses/MN/MN/Regresion.xlsx
+++ b/courses/MN/MN/Regresion.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16000" windowHeight="11460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>x</t>
   </si>
@@ -48,11 +49,62 @@
   <si>
     <t>x^2</t>
   </si>
+  <si>
+    <t>Suma</t>
+  </si>
+  <si>
+    <t>Promedio</t>
+  </si>
+  <si>
+    <t>ymod</t>
+  </si>
+  <si>
+    <t>(y-ymod)^2</t>
+  </si>
+  <si>
+    <t>(y-y_)^2</t>
+  </si>
+  <si>
+    <t>St</t>
+  </si>
+  <si>
+    <t>Sr</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>x^3</t>
+  </si>
+  <si>
+    <t>x^4</t>
+  </si>
+  <si>
+    <t>x^2y</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Matriz inversa</t>
+  </si>
+  <si>
+    <t>Matriz original</t>
+  </si>
+  <si>
+    <t>Multiplicar (inv(A)*b)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -95,7 +147,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -121,11 +173,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="61">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -138,6 +230,24 @@
     <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -150,6 +260,24 @@
     <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -313,11 +441,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109801256"/>
-        <c:axId val="2109764152"/>
+        <c:axId val="2076766664"/>
+        <c:axId val="2076769784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2109801256"/>
+        <c:axId val="2076766664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -327,7 +455,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109764152"/>
+        <c:crossAx val="2076769784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -335,7 +463,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109764152"/>
+        <c:axId val="2076769784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -346,7 +474,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109801256"/>
+        <c:crossAx val="2076766664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -504,11 +632,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132373816"/>
-        <c:axId val="-2134624728"/>
+        <c:axId val="2076856232"/>
+        <c:axId val="2076859096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132373816"/>
+        <c:axId val="2076856232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,12 +646,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2134624728"/>
+        <c:crossAx val="2076859096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2134624728"/>
+        <c:axId val="2076859096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,7 +662,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132373816"/>
+        <c:crossAx val="2076856232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -687,11 +815,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2063910248"/>
-        <c:axId val="2064411816"/>
+        <c:axId val="2076886056"/>
+        <c:axId val="2076888920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2063910248"/>
+        <c:axId val="2076886056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -701,12 +829,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064411816"/>
+        <c:crossAx val="2076888920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2064411816"/>
+        <c:axId val="2076888920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -717,7 +845,194 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2063910248"/>
+        <c:crossAx val="2076886056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.000211053865180433"/>
+                  <c:y val="-0.06"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="2400"/>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2099255560"/>
+        <c:axId val="2099296952"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2099255560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2099296952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2099296952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2099255560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -826,6 +1141,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1158,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1203,11 +1553,11 @@
         <v>5.32</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D11" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D9" si="0">B3*C3</f>
         <v>10.64</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E10" si="1">B3^2</f>
+        <f t="shared" ref="E3:E9" si="1">B3^2</f>
         <v>4</v>
       </c>
     </row>
@@ -1587,4 +1937,683 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <f>B2*C2</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <f>B2^2</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <f>$B$16*B2+$B$15</f>
+        <v>-0.55555555555555514</v>
+      </c>
+      <c r="G2" s="2">
+        <f>(C2-F2)^2</f>
+        <v>2.4197530864197518</v>
+      </c>
+      <c r="H2" s="2">
+        <f>(C2-$C$12)^2</f>
+        <v>18.299382716049383</v>
+      </c>
+      <c r="I2">
+        <f>B2^3</f>
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <f>B2^4</f>
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>E2*C2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D10" si="0">B3*C3</f>
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E10" si="1">B3^2</f>
+        <v>4</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F11" si="2">$B$16*B3+$B$15</f>
+        <v>0.90277777777777812</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G10" si="3">(C3-F3)^2</f>
+        <v>0.35667438271604895</v>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H10" si="4">(C3-$C$12)^2</f>
+        <v>14.271604938271604</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I10" si="5">B3^3</f>
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J10" si="6">B3^4</f>
+        <v>16</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K10" si="7">E3*C3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="2"/>
+        <v>2.3611111111111116</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="3"/>
+        <v>0.13040123456790159</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="4"/>
+        <v>10.743827160493826</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="6"/>
+        <v>81</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="7"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="2"/>
+        <v>3.8194444444444446</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="3"/>
+        <v>0.67148919753086456</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="4"/>
+        <v>5.1882716049382713</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="5"/>
+        <v>64</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="6"/>
+        <v>256</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="7"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="2"/>
+        <v>5.2777777777777777</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="3"/>
+        <v>1.6327160493827158</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="4"/>
+        <v>1.6327160493827158</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="5"/>
+        <v>125</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="6"/>
+        <v>625</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="2"/>
+        <v>6.7361111111111116</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="3"/>
+        <v>3.0140817901234587</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="4"/>
+        <v>7.7160493827160434E-2</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="5"/>
+        <v>216</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="6"/>
+        <v>1296</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="7"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="2"/>
+        <v>8.1944444444444429</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="3"/>
+        <v>3.7808641975308026E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="4"/>
+        <v>7.4104938271604945</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="5"/>
+        <v>343</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="6"/>
+        <v>2401</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="7"/>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="2"/>
+        <v>9.6527777777777786</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12056327160493772</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="4"/>
+        <v>22.299382716049383</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="5"/>
+        <v>512</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="6"/>
+        <v>4096</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="7"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="2"/>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="3"/>
+        <v>3.5679012345679029</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="4"/>
+        <v>59.632716049382715</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="5"/>
+        <v>729</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="6"/>
+        <v>6561</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="7"/>
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <f>SUM(B2:B10)</f>
+        <v>45</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" ref="C11:E11" si="8">SUM(C2:C10)</f>
+        <v>47.5</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="8"/>
+        <v>325</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="8"/>
+        <v>285</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="2"/>
+        <v>63.611111111111114</v>
+      </c>
+      <c r="G11" s="2">
+        <f>SUM(G2:G10)</f>
+        <v>11.951388888888893</v>
+      </c>
+      <c r="H11" s="2">
+        <f>SUM(H2:H10)</f>
+        <v>139.55555555555554</v>
+      </c>
+      <c r="I11" s="2">
+        <f>SUM(I2:I10)</f>
+        <v>2025</v>
+      </c>
+      <c r="J11" s="2">
+        <f>SUM(J2:J10)</f>
+        <v>15333</v>
+      </c>
+      <c r="K11" s="2">
+        <f>SUM(K2:K10)</f>
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f>AVERAGE(B2:B10)</f>
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <f>AVERAGE(C2:C10)</f>
+        <v>5.2777777777777777</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <f>COUNT(B2:B10)</f>
+        <v>9</v>
+      </c>
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <f>C12-B16*B12</f>
+        <v>-2.0138888888888884</v>
+      </c>
+      <c r="K15" t="s">
+        <v>5</v>
+      </c>
+      <c r="L15" t="s">
+        <v>6</v>
+      </c>
+      <c r="M15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <f>(B14*D11-B11*C11)/(B14*E11-B11^2)</f>
+        <v>1.4583333333333333</v>
+      </c>
+      <c r="K16">
+        <f>B14</f>
+        <v>9</v>
+      </c>
+      <c r="L16">
+        <f>B11</f>
+        <v>45</v>
+      </c>
+      <c r="M16">
+        <f>E11</f>
+        <v>285</v>
+      </c>
+      <c r="N16">
+        <f>C11</f>
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="K17">
+        <f>L16</f>
+        <v>45</v>
+      </c>
+      <c r="L17">
+        <f>M16</f>
+        <v>285</v>
+      </c>
+      <c r="M17" s="2">
+        <f>I11</f>
+        <v>2025</v>
+      </c>
+      <c r="N17">
+        <f>D11</f>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <f>H11</f>
+        <v>139.55555555555554</v>
+      </c>
+      <c r="K18">
+        <f>L17</f>
+        <v>285</v>
+      </c>
+      <c r="L18" s="2">
+        <f>M17</f>
+        <v>2025</v>
+      </c>
+      <c r="M18" s="2">
+        <f>J11</f>
+        <v>15333</v>
+      </c>
+      <c r="N18" s="2">
+        <f>K11</f>
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <f>G11</f>
+        <v>11.951388888888893</v>
+      </c>
+      <c r="K19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <f>(H11-G11)/H11</f>
+        <v>0.91436106687898089</v>
+      </c>
+      <c r="K20" t="s">
+        <v>5</v>
+      </c>
+      <c r="L20" t="s">
+        <v>6</v>
+      </c>
+      <c r="M20" t="s">
+        <v>20</v>
+      </c>
+      <c r="N20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="K21">
+        <f t="array" ref="K21:M23">MINVERSE(K16:M18)</f>
+        <v>1.6190476190475955</v>
+      </c>
+      <c r="L21">
+        <v>-0.6785714285714165</v>
+      </c>
+      <c r="M21">
+        <v>5.9523809523808431E-2</v>
+      </c>
+      <c r="N21">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="K22">
+        <v>-0.67857142857141739</v>
+      </c>
+      <c r="L22">
+        <v>0.34134199134198562</v>
+      </c>
+      <c r="M22">
+        <v>-3.246753246753193E-2</v>
+      </c>
+      <c r="N22">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="K23">
+        <v>5.952380952380848E-2</v>
+      </c>
+      <c r="L23">
+        <v>-3.2467532467531937E-2</v>
+      </c>
+      <c r="M23">
+        <v>3.2467532467531967E-3</v>
+      </c>
+      <c r="N23">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="K24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="J25" t="s">
+        <v>5</v>
+      </c>
+      <c r="K25">
+        <f t="array" ref="K25:K27">MMULT(K21:M23,N21:N23)</f>
+        <v>1.4880952380953829</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="J26" t="s">
+        <v>6</v>
+      </c>
+      <c r="K26">
+        <v>-0.45183982683984425</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="J27" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27">
+        <v>0.19101731601731586</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>